<commit_message>
modify loading, empty, locales
</commit_message>
<xml_diff>
--- a/src/localesjs/moneygone_locales.xlsx
+++ b/src/localesjs/moneygone_locales.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="169">
   <si>
     <t>key</t>
   </si>
@@ -505,14 +505,26 @@
     <t>這個月會花多少勒...</t>
   </si>
   <si>
-    <t>how much will spend this month...</t>
+    <t>How much will spend this month...</t>
+  </si>
+  <si>
+    <t>LC_LOADING</t>
+  </si>
+  <si>
+    <t>載入中...</t>
+  </si>
+  <si>
+    <t>Loading...</t>
+  </si>
+  <si>
+    <t>読み込み中...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -522,6 +534,10 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -538,12 +554,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1518,10 +1537,22 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B43,""ZH-TW"",""ZH-CN"")"),"载入中...")</f>
+        <v>载入中...</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1"/>

</xml_diff>